<commit_message>
appli vba version 1.0 operationnel
Premiere version 1.0 operationnel .
Le code n'est pas encore parfait mais c'est une version 1.0
La premiere application réalisé en VBA
Amélioré en utilisant plus de modules de classes
</commit_message>
<xml_diff>
--- a/suiviePatins.xlsx
+++ b/suiviePatins.xlsx
@@ -1281,7 +1281,9 @@
       <c r="F21" s="30"/>
       <c r="G21" s="31"/>
       <c r="H21" s="30"/>
-      <c r="I21" s="32"/>
+      <c r="I21" s="32">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
@@ -1318,8 +1320,12 @@
       <c r="E23" s="13"/>
       <c r="F23" s="12"/>
       <c r="G23" s="13"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="14"/>
+      <c r="H23" s="12">
+        <v>30</v>
+      </c>
+      <c r="I23" s="14">
+        <v>250</v>
+      </c>
     </row>
     <row r="24" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
@@ -1327,12 +1333,18 @@
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="12"/>
+      <c r="D24" s="12">
+        <v>1</v>
+      </c>
       <c r="E24" s="13"/>
       <c r="F24" s="12"/>
       <c r="G24" s="13"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="14"/>
+      <c r="H24" s="12">
+        <v>40</v>
+      </c>
+      <c r="I24" s="14">
+        <v>20</v>
+      </c>
     </row>
     <row r="25" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
@@ -1472,7 +1484,7 @@
       </c>
       <c r="D35" s="20">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E35" s="21">
         <f t="shared" si="0"/>
@@ -1488,11 +1500,11 @@
       </c>
       <c r="H35" s="20">
         <f t="shared" si="0"/>
-        <v>805</v>
+        <v>875</v>
       </c>
       <c r="I35" s="22">
         <f t="shared" si="0"/>
-        <v>320</v>
+        <v>610</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -1506,7 +1518,7 @@
       <c r="C36" s="42"/>
       <c r="D36" s="43">
         <f>E35-D35</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="E36" s="44"/>
       <c r="F36" s="43">
@@ -1516,7 +1528,7 @@
       <c r="G36" s="44"/>
       <c r="H36" s="43">
         <f>I35-H35</f>
-        <v>-485</v>
+        <v>-265</v>
       </c>
       <c r="I36" s="44"/>
     </row>
@@ -1531,7 +1543,7 @@
       <c r="C37" s="34"/>
       <c r="D37" s="33">
         <f>janvier!D37+D36</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="E37" s="34"/>
       <c r="F37" s="33">
@@ -1541,7 +1553,7 @@
       <c r="G37" s="34"/>
       <c r="H37" s="33">
         <f>janvier!H37+H36</f>
-        <v>-467</v>
+        <v>-247</v>
       </c>
       <c r="I37" s="34"/>
     </row>
@@ -1581,7 +1593,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37 F37">
+  <conditionalFormatting sqref="F37 D37">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2153,7 +2165,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F37 D37">
+  <conditionalFormatting sqref="D37 F37">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2707,7 +2719,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F37 D37">
+  <conditionalFormatting sqref="D37 F37">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>